<commit_message>
Modified total bcq nomination Excel file
</commit_message>
<xml_diff>
--- a/total_bcq_nomination.xlsx
+++ b/total_bcq_nomination.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,11 +444,6 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>PEDC</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>TOTAL_BCQ</t>
         </is>
       </c>
@@ -458,19 +453,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C2" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>22500</v>
+        <v>57000</v>
       </c>
     </row>
     <row r="3">
@@ -478,19 +470,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C3" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>22500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="4">
@@ -498,19 +487,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C4" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>22500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="5">
@@ -518,19 +504,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C5" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>22500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="6">
@@ -538,19 +521,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C6" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>22500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="7">
@@ -558,19 +538,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C7" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D7" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>32500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="8">
@@ -584,13 +561,10 @@
         <v>10000</v>
       </c>
       <c r="D8" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>32500</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="9">
@@ -598,19 +572,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C9" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D9" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>32500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="10">
@@ -618,19 +589,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C10" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D10" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>42500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="11">
@@ -638,19 +606,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C11" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D11" t="n">
         <v>20000</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>42500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="12">
@@ -658,19 +623,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C12" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D12" t="n">
         <v>20000</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>42500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="13">
@@ -678,19 +640,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C13" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D13" t="n">
         <v>20000</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>42500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="14">
@@ -698,19 +657,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C14" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D14" t="n">
         <v>20000</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>42500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="15">
@@ -718,19 +674,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C15" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D15" t="n">
         <v>20000</v>
       </c>
       <c r="E15" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F15" t="n">
-        <v>52500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="16">
@@ -738,19 +691,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C16" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D16" t="n">
         <v>20000</v>
       </c>
       <c r="E16" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F16" t="n">
-        <v>52500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="17">
@@ -758,19 +708,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C17" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D17" t="n">
         <v>20000</v>
       </c>
       <c r="E17" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F17" t="n">
-        <v>52500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="18">
@@ -787,10 +734,7 @@
         <v>20000</v>
       </c>
       <c r="E18" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F18" t="n">
-        <v>75000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="19">
@@ -807,10 +751,7 @@
         <v>20000</v>
       </c>
       <c r="E19" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F19" t="n">
-        <v>75000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="20">
@@ -827,10 +768,7 @@
         <v>20000</v>
       </c>
       <c r="E20" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F20" t="n">
-        <v>75000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="21">
@@ -847,10 +785,7 @@
         <v>20000</v>
       </c>
       <c r="E21" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F21" t="n">
-        <v>75000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="22">
@@ -867,10 +802,7 @@
         <v>20000</v>
       </c>
       <c r="E22" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F22" t="n">
-        <v>75000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="23">
@@ -887,10 +819,7 @@
         <v>20000</v>
       </c>
       <c r="E23" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F23" t="n">
-        <v>75000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="24">
@@ -898,19 +827,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C24" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D24" t="n">
         <v>20000</v>
       </c>
       <c r="E24" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F24" t="n">
-        <v>52500</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="25">
@@ -918,19 +844,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>12500</v>
+        <v>25000</v>
       </c>
       <c r="C25" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D25" t="n">
         <v>20000</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>42500</v>
+        <v>65000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>